<commit_message>
Deleted first row in 4736, adjusted subno column of 682 from 692 to match folder number
</commit_message>
<xml_diff>
--- a/data/s682_1/DD_682.xlsx
+++ b/data/s682_1/DD_682.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tug47820\Downloads\data\data\s682_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tul67061\Documents\GitHub\accomodation\data\s682_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23640" windowHeight="10755"/>
   </bookViews>
   <sheets>
     <sheet name="DD_682" sheetId="1" r:id="rId1"/>
@@ -1091,13 +1091,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BR54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1309,12 +1309,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>70</v>
       </c>
       <c r="B2">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1452,12 +1452,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
       <c r="B3">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1595,12 +1595,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>70</v>
       </c>
       <c r="B4">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1762,12 +1762,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
       <c r="B5">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1932,12 +1932,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>70</v>
       </c>
       <c r="B6">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2105,12 +2105,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>70</v>
       </c>
       <c r="B7">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2281,12 +2281,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>70</v>
       </c>
       <c r="B8">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2457,12 +2457,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>70</v>
       </c>
       <c r="B9">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -2633,12 +2633,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
       <c r="B10">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -2809,12 +2809,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>70</v>
       </c>
       <c r="B11">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2985,12 +2985,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>70</v>
       </c>
       <c r="B12">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -3161,12 +3161,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>70</v>
       </c>
       <c r="B13">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -3337,12 +3337,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>70</v>
       </c>
       <c r="B14">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -3513,12 +3513,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>70</v>
       </c>
       <c r="B15">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -3689,12 +3689,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>70</v>
       </c>
       <c r="B16">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -3865,12 +3865,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>70</v>
       </c>
       <c r="B17">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -4041,12 +4041,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>70</v>
       </c>
       <c r="B18">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -4217,12 +4217,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>70</v>
       </c>
       <c r="B19">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -4393,12 +4393,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>70</v>
       </c>
       <c r="B20">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -4569,12 +4569,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>70</v>
       </c>
       <c r="B21">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -4745,12 +4745,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>70</v>
       </c>
       <c r="B22">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -4921,12 +4921,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>70</v>
       </c>
       <c r="B23">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -5097,12 +5097,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>70</v>
       </c>
       <c r="B24">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -5273,12 +5273,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>70</v>
       </c>
       <c r="B25">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -5449,12 +5449,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>70</v>
       </c>
       <c r="B26">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -5625,12 +5625,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>70</v>
       </c>
       <c r="B27">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -5801,12 +5801,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>70</v>
       </c>
       <c r="B28">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -5977,12 +5977,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>70</v>
       </c>
       <c r="B29">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -6153,12 +6153,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>70</v>
       </c>
       <c r="B30">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -6329,12 +6329,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>70</v>
       </c>
       <c r="B31">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -6505,12 +6505,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>70</v>
       </c>
       <c r="B32">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -6681,12 +6681,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>70</v>
       </c>
       <c r="B33">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -6857,12 +6857,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>70</v>
       </c>
       <c r="B34">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -7033,12 +7033,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>70</v>
       </c>
       <c r="B35">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -7209,12 +7209,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>70</v>
       </c>
       <c r="B36">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -7385,12 +7385,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>70</v>
       </c>
       <c r="B37">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -7561,12 +7561,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>70</v>
       </c>
       <c r="B38">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -7737,12 +7737,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>70</v>
       </c>
       <c r="B39">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -7913,12 +7913,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>70</v>
       </c>
       <c r="B40">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -8089,12 +8089,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>70</v>
       </c>
       <c r="B41">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -8265,12 +8265,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>70</v>
       </c>
       <c r="B42">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -8441,12 +8441,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>70</v>
       </c>
       <c r="B43">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -8617,12 +8617,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>70</v>
       </c>
       <c r="B44">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -8793,12 +8793,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>70</v>
       </c>
       <c r="B45">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -8969,12 +8969,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>70</v>
       </c>
       <c r="B46">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -9145,12 +9145,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>70</v>
       </c>
       <c r="B47">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -9321,12 +9321,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>70</v>
       </c>
       <c r="B48">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -9497,12 +9497,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>70</v>
       </c>
       <c r="B49">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -9673,12 +9673,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>70</v>
       </c>
       <c r="B50">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -9849,12 +9849,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>70</v>
       </c>
       <c r="B51">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -10025,12 +10025,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>70</v>
       </c>
       <c r="B52">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -10201,12 +10201,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>70</v>
       </c>
       <c r="B53">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -10377,12 +10377,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>70</v>
       </c>
       <c r="B54">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C54">
         <v>1</v>

</xml_diff>